<commit_message>
Updated research project excel file (Removed amount alongside funding agency) and date added
</commit_message>
<xml_diff>
--- a/research-projects.xlsx
+++ b/research-projects.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4518248c6cd0c0d5/Desktop/CSPIT_NEW_2024/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\motat\OneDrive\Desktop\CSPIT_NEW_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{537CB467-00B3-4A00-B5F4-64C48977B08A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{961742C5-0F60-4085-9CF2-B19FC5543723}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C29ECE17-2F4F-4AAF-A072-4D8807BEDE9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{341EFF14-0348-4CC8-873A-B058F927C9C9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="132">
   <si>
     <t>Sr No</t>
   </si>
@@ -222,171 +222,6 @@
     <t>Funding Agency</t>
   </si>
   <si>
-    <t>CHARUSAT - 300000.00 (INR)</t>
-  </si>
-  <si>
-    <t>CHARUSAT - 150000.00 (INR)</t>
-  </si>
-  <si>
-    <t>CHARUSAT - 70000.00 (INR)</t>
-  </si>
-  <si>
-    <t>CHARUSAT - 200000.00 (INR)</t>
-  </si>
-  <si>
-    <t>CHARUSAT - 62360.00 (INR)</t>
-  </si>
-  <si>
-    <t>CHARUSAT - 644300.00 (INR)</t>
-  </si>
-  <si>
-    <t>CHARUSAT - 55750.00 (INR)</t>
-  </si>
-  <si>
-    <t>CHARUSAT - 25000.00 (INR)</t>
-  </si>
-  <si>
-    <t>CHARUSAT - 75000.00 (INR)</t>
-  </si>
-  <si>
-    <t>EDUNET FOUNDATION - 1600000.00 (INR)</t>
-  </si>
-  <si>
-    <t>CHARUSAT - 455000.00 (INR)</t>
-  </si>
-  <si>
-    <t>CHARUSAT - 30800000.00 (INR)</t>
-  </si>
-  <si>
-    <t>GUJARAT COUNCIL ON SCIENCE AND TECHNOLOGY ( GUJCOST ) - 105000.00 (INR)</t>
-  </si>
-  <si>
-    <t>GANDHINAGAR UNIVERSITY - 1750000.00 (INR)</t>
-  </si>
-  <si>
-    <t>CHARUSAT - 250000.00 (INR)</t>
-  </si>
-  <si>
-    <t>CHARUSAT - 375000.00 (INR)</t>
-  </si>
-  <si>
-    <t>CHARUSAT - 0.00 (INR)</t>
-  </si>
-  <si>
-    <t>BHAIKAKA UNIVERSITY - 0.00 (INR)</t>
-  </si>
-  <si>
-    <t>GUJARAT COUNCIL ON SCIENCE AND TECHNOLOGY (GUJCOST) - 250000.00 (INR)</t>
-  </si>
-  <si>
-    <t>STUDENT STARTUP AND INNOVATION POLICY (SSIP) - 70000.00 (INR), CHARUSAT STARTUP AND INNOVATION CENTRE(CSIC),CHARUSAT - 15000.00 (INR)</t>
-  </si>
-  <si>
-    <t>STUDENT STARTUP AND INNOVATION POLICY (SSIP) - 10000.00 (INR), CHARUSAT STARTUP AND INNOVATION CENTRE (CSIC), CHARUSAT - 10000.00 (INR)</t>
-  </si>
-  <si>
-    <t>METTA EV PRIVATE LIMITED - 35400.00 (INR)</t>
-  </si>
-  <si>
-    <t>EDUNET FOUNDATION, SAP - 76445.00 (INR)</t>
-  </si>
-  <si>
-    <t>KARMA TIME FOUNDATION - 250100.00 (INR)</t>
-  </si>
-  <si>
-    <t>GENUIN CODEBASE LLP - 127440.00 (INR)</t>
-  </si>
-  <si>
-    <t>NANDESARI ENVIRONMENT CONTROL LIMITED - 50000.00 (INR)</t>
-  </si>
-  <si>
-    <t>GUJARAT COUNCIL ON SCIENCE AND TECHNOLOGY - 50000.00 (INR)</t>
-  </si>
-  <si>
-    <t>GUJARAT COUNCIL ON SCIENCE &amp; TECHNOLOGY (GUJCOST) - 50000.00 (INR)</t>
-  </si>
-  <si>
-    <t>CHARUSAT - 120000.00 (INR)</t>
-  </si>
-  <si>
-    <t>CHARUSAT - 240000.00 (INR)</t>
-  </si>
-  <si>
-    <t>CHARUSAT - 100000.00 (INR)</t>
-  </si>
-  <si>
-    <t>CHARUSAT - 320000.00 (INR)</t>
-  </si>
-  <si>
-    <t>CHARUSAT - 500000.00 (INR)</t>
-  </si>
-  <si>
-    <t>CHARUSAT - 50000.00 (INR)</t>
-  </si>
-  <si>
-    <t>VALLABH VIDHYA NAGAR TOWN CLUB - 141600.00 (INR)</t>
-  </si>
-  <si>
-    <t>ROTOMAG MOTORS &amp; CONTROLS PVT. LTD. - 59000.00 (INR)</t>
-  </si>
-  <si>
-    <t>DST- SERB - 1617000.00 (INR)</t>
-  </si>
-  <si>
-    <t>CHARUSAT - 363000.00 (INR)</t>
-  </si>
-  <si>
-    <t>CHARUSAT - 70176.00 (INR)</t>
-  </si>
-  <si>
-    <t>CHARUSAT - 190000.00 (INR)</t>
-  </si>
-  <si>
-    <t>NVIDIA - 175000.00 (INR)</t>
-  </si>
-  <si>
-    <t>GUJARAT COUNCIL ON SCIENCE AND TECHNOLOGY - 1480900.00 (INR)</t>
-  </si>
-  <si>
-    <t>AICTE - 508800.00 (INR)</t>
-  </si>
-  <si>
-    <t>CHARUSAT - 51274.00 (INR)</t>
-  </si>
-  <si>
-    <t>GUJARAT COUNCIL ON SCIENCE &amp; TECHNOLOGY (GUJCOST) - 150000.00 (INR)</t>
-  </si>
-  <si>
-    <t>POINTBASES - 150000.00 (INR)</t>
-  </si>
-  <si>
-    <t>GUJARAT POLLTION CONTROL BOARD - 4986050.00 (INR)</t>
-  </si>
-  <si>
-    <t>SCIENCE AND ENGINEERING RESEARCH BOARD (SERB) - DEPARTMENT OF SCIENCE &amp; TECHNOLOGY (DST) - 825000.00 (INR)</t>
-  </si>
-  <si>
-    <t>CHARUSAT - 430000.00 (INR)</t>
-  </si>
-  <si>
-    <t>CHARUSAT - 168000.00 (INR)</t>
-  </si>
-  <si>
-    <t>CHARUSAT - 35000.00 (INR)</t>
-  </si>
-  <si>
-    <t>CHARUSAT - 85000.00 (INR)</t>
-  </si>
-  <si>
-    <t>CHARUSAT - 58500.00 (INR)</t>
-  </si>
-  <si>
-    <t>CHARUSAT - 84800.00 (INR)</t>
-  </si>
-  <si>
-    <t>INDIAN SPACE RESEARCH ORGANIZATION - 4330960.00 (INR)</t>
-  </si>
-  <si>
     <t>Total Fund Received during the Period</t>
   </si>
   <si>
@@ -526,6 +361,75 @@
   </si>
   <si>
     <t>TRUSHIT KIRTIKUMAR UPADHYAYA - CHARUSAT - PI, KILLOL VISHNUPRASAD PANDYA - CHARUSAT - Co-PI, UPESH PARBHUBHAI PATEL - CHARUSAT - Co-PI</t>
+  </si>
+  <si>
+    <t>CHARUSAT</t>
+  </si>
+  <si>
+    <t>EDUNET FOUNDATION</t>
+  </si>
+  <si>
+    <t>GUJARAT COUNCIL ON SCIENCE AND TECHNOLOGY (GUJCOST)</t>
+  </si>
+  <si>
+    <t>GANDHINAGAR UNIVERSITY</t>
+  </si>
+  <si>
+    <t>BHAIKAKA UNIVERSITY</t>
+  </si>
+  <si>
+    <t>STUDENT STARTUP AND INNOVATION POLICY (SSIP), CHARUSAT STARTUP AND INNOVATION CENTRE (CSIC), CHARUSAT</t>
+  </si>
+  <si>
+    <t>METTA EV PRIVATE LIMITED</t>
+  </si>
+  <si>
+    <t>EDUNET FOUNDATION, SAP</t>
+  </si>
+  <si>
+    <t>KARMA TIME FOUNDATION</t>
+  </si>
+  <si>
+    <t>GENUIN CODEBASE LLP</t>
+  </si>
+  <si>
+    <t>NANDESARI ENVIRONMENT CONTROL LIMITED</t>
+  </si>
+  <si>
+    <t>GUJARAT COUNCIL ON SCIENCE AND TECHNOLOGY</t>
+  </si>
+  <si>
+    <t>GUJARAT COUNCIL ON SCIENCE &amp; TECHNOLOGY (GUJCOST)</t>
+  </si>
+  <si>
+    <t>VALLABH VIDHYA NAGAR TOWN CLUB</t>
+  </si>
+  <si>
+    <t>ROTOMAG MOTORS &amp; CONTROLS PVT. LTD.</t>
+  </si>
+  <si>
+    <t>DST- SERB</t>
+  </si>
+  <si>
+    <t>NVIDIA</t>
+  </si>
+  <si>
+    <t>AICTE</t>
+  </si>
+  <si>
+    <t>POINTBASES</t>
+  </si>
+  <si>
+    <t>GUJARAT POLLUTION CONTROL BOARD</t>
+  </si>
+  <si>
+    <t>SCIENCE AND ENGINEERING RESEARCH BOARD (SERB), DEPARTMENT OF SCIENCE &amp; TECHNOLOGY (DST)</t>
+  </si>
+  <si>
+    <t>INDIAN SPACE RESEARCH ORGANIZATION</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -856,7 +760,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -973,6 +877,32 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
@@ -1031,12 +961,19 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="18" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1095,10 +1032,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1398,10 +1331,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F478AB01-734C-4F31-9ADF-76A14C6FE5CE}">
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="312" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1411,7 +1344,7 @@
     <col min="5" max="5" width="36.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1422,1050 +1355,1237 @@
         <v>61</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>117</v>
+        <v>62</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>62</v>
+      <c r="C2" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D2" s="2">
         <v>300000</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+      <c r="F2" s="5">
+        <v>44156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>63</v>
+      <c r="C3" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D3" s="2">
         <v>150000</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+      <c r="F3" s="5">
+        <v>44885</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>64</v>
+      <c r="C4" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D4" s="2">
         <v>70000</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+      <c r="F4" s="5">
+        <v>44631</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>65</v>
+      <c r="C5" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D5" s="2">
         <v>200000</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+      <c r="F5" s="5">
+        <v>44651</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>66</v>
+      <c r="C6" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D6" s="2">
         <v>62360</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+      <c r="F6" s="5">
+        <v>44712</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>67</v>
+      <c r="C7" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D7" s="2">
         <v>644300</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+      <c r="F7" s="5">
+        <v>44712</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>68</v>
+      <c r="C8" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D8" s="2">
         <v>55750</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+      <c r="F8" s="5">
+        <v>44681</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>69</v>
+      <c r="C9" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D9" s="2">
         <v>25000</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="F9" s="5">
+        <v>45766</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>70</v>
+      <c r="C10" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D10" s="2">
         <v>75000</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+      <c r="F10" s="5">
+        <v>44787</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>71</v>
+      <c r="C11" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="D11" s="2">
         <v>1600000</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+      <c r="F11" s="5">
+        <v>45291</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>72</v>
+      <c r="C12" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D12" s="2">
         <v>455000</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="F12" s="5">
+        <v>45138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>73</v>
+      <c r="C13" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D13" s="2">
         <v>30800000</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+      <c r="F13" s="5">
+        <v>45154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>74</v>
+      <c r="C14" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="D14" s="2">
         <v>105000</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+      <c r="F14" s="5">
+        <v>42914</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>75</v>
+      <c r="C15" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="D15" s="2">
         <v>1750000</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="F15" s="5">
+        <v>45138</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>76</v>
+      <c r="C16" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D16" s="2">
         <v>250000</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="F16" s="5">
+        <v>45138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>77</v>
+      <c r="C17" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D17" s="2">
         <v>375000</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="F17" s="5">
+        <v>45138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>78</v>
+      <c r="C18" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D18" s="2">
         <v>0</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+      <c r="F18" s="5">
+        <v>45230</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>79</v>
+      <c r="C19" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="D19" s="2">
         <v>0</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="F19" s="5">
+        <v>45230</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>80</v>
+      <c r="C20" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="D20" s="2">
         <v>250000</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="F20" s="5">
+        <v>45260</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>69</v>
+      <c r="C21" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D21" s="2">
         <v>25000</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="F21" s="5">
+        <v>45291</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>70</v>
+      <c r="C22" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D22" s="2">
         <v>75000</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="F22" s="5">
+        <v>45291</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>81</v>
+      <c r="C23" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="D23" s="2">
         <v>85000</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+      <c r="F23" s="5">
+        <v>46387</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>82</v>
+      <c r="C24" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="D24" s="2">
         <v>20000</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+      <c r="F24" s="5">
+        <v>45657</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>83</v>
+      <c r="C25" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="D25" s="2">
         <v>35400</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="F25" s="5">
+        <v>45312</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>84</v>
+      <c r="C26" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="D26" s="2">
         <v>76445</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+      <c r="F26" s="5">
+        <v>46022</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>85</v>
+      <c r="C27" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="D27" s="2">
         <v>250100</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+      <c r="F27" s="5">
+        <v>45838</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>86</v>
+      <c r="C28" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="D28" s="2">
         <v>127440</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="F28" s="5">
+        <v>45747</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>87</v>
+      <c r="C29" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="D29" s="2">
         <v>50000</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="F29" s="5">
+        <v>45481</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>88</v>
+      <c r="C30" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="D30" s="2">
         <v>50000</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="F30" s="5">
+        <v>45877</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>88</v>
+      <c r="C31" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="D31" s="2">
         <v>50000</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="F31" s="5">
+        <v>45877</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>89</v>
+      <c r="C32" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="D32" s="2">
         <v>50000</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+      <c r="F32" s="5">
+        <v>45591</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>90</v>
+      <c r="C33" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D33" s="2">
         <v>120000</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+      <c r="F33" s="5">
+        <v>44265</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>91</v>
+      <c r="C34" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D34" s="2">
         <v>240000</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+      <c r="F34" s="5">
+        <v>44158</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>92</v>
+      <c r="C35" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D35" s="2">
         <v>100000</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+      <c r="F35" s="5">
+        <v>44889</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>93</v>
+      <c r="C36" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D36" s="2">
         <v>320000</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="F36" s="5">
+        <v>44286</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>94</v>
+      <c r="C37" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D37" s="2">
         <v>500000</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="F37" s="5">
+        <v>44815</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>95</v>
+      <c r="C38" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D38" s="2">
         <v>50000</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+      <c r="F38" s="5">
+        <v>44926</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>92</v>
+      <c r="C39" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D39" s="2">
         <v>100000</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+      <c r="F39" s="5">
+        <v>44524</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>65</v>
+      <c r="C40" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D40" s="2">
         <v>200000</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+      <c r="F40" s="5">
+        <v>44156</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>96</v>
+      <c r="C41" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="D41" s="2">
         <v>141600</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="F41" s="5">
+        <v>44407</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>97</v>
+      <c r="C42" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="D42" s="2">
         <v>59000</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+      <c r="F42" s="5">
+        <v>44377</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>98</v>
+      <c r="C43" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="D43" s="2">
         <v>1617000</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+      <c r="F43" s="5">
+        <v>44424</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>99</v>
+      <c r="C44" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D44" s="2">
         <v>363000</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+      <c r="F44" s="5">
+        <v>44347</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>100</v>
+      <c r="C45" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D45" s="2">
         <v>70176</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+      <c r="F45" s="5">
+        <v>44651</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>92</v>
+      <c r="C46" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D46" s="2">
         <v>100000</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+      <c r="F46" s="5">
+        <v>44651</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C47" s="2" t="s">
-        <v>101</v>
+      <c r="C47" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D47" s="2">
         <v>190000</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+      <c r="F47" s="5">
+        <v>45351</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>102</v>
+      <c r="C48" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="D48" s="2">
         <v>175000</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+      <c r="F48" s="5">
+        <v>44560</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>103</v>
+      <c r="C49" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="D49" s="2">
         <v>1480900</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="F49" s="5">
+        <v>44742</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C50" s="2" t="s">
-        <v>104</v>
+      <c r="C50" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="D50" s="2">
         <v>508800</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="F50" s="5">
+        <v>44313</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C51" s="2" t="s">
-        <v>105</v>
+      <c r="C51" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D51" s="2">
         <v>51274</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="F51" s="5">
+        <v>44266</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>106</v>
+      <c r="C52" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="D52" s="2">
         <v>150000</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+      <c r="F52" s="5">
+        <v>44196</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>107</v>
+      <c r="C53" s="3" t="s">
+        <v>127</v>
       </c>
       <c r="D53" s="2">
         <v>150000</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="F53" s="5">
+        <v>44448</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C54" s="2" t="s">
-        <v>108</v>
+      <c r="C54" s="3" t="s">
+        <v>128</v>
       </c>
       <c r="D54" s="2">
         <v>4986050</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+      <c r="F54" s="5">
+        <v>44286</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>109</v>
+      <c r="C55" s="3" t="s">
+        <v>129</v>
       </c>
       <c r="D55" s="2">
         <v>825000</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+      <c r="F55" s="5">
+        <v>45275</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>110</v>
+      <c r="C56" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D56" s="2">
         <v>430000</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+      <c r="F56" s="5">
+        <v>45016</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>111</v>
+      <c r="C57" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D57" s="2">
         <v>168000</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+      <c r="F57" s="5">
+        <v>45107</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C58" s="2" t="s">
-        <v>112</v>
+      <c r="C58" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D58" s="2">
         <v>35000</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+      <c r="F58" s="5">
+        <v>44651</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C59" s="2" t="s">
-        <v>113</v>
+      <c r="C59" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D59" s="2">
         <v>85000</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+      <c r="F59" s="5">
+        <v>44651</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C60" s="2" t="s">
-        <v>114</v>
+      <c r="C60" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D60" s="2">
         <v>58500</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="F60" s="5">
+        <v>44651</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C61" s="2" t="s">
-        <v>115</v>
+      <c r="C61" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="D61" s="2">
         <v>84800</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+      <c r="F61" s="5">
+        <v>44773</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C62" s="2" t="s">
-        <v>116</v>
+      <c r="C62" s="3" t="s">
+        <v>130</v>
       </c>
       <c r="D62" s="2">
         <v>4330960</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>163</v>
+        <v>108</v>
+      </c>
+      <c r="F62" s="5">
+        <v>45353</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>